<commit_message>
rerun for autotime timestamps
</commit_message>
<xml_diff>
--- a/cabinet.xlsx
+++ b/cabinet.xlsx
@@ -642,7 +642,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Bachelor of Arts in History and Politics, Bachelor of Laws (first-class honours)</t>
+          <t>Bachelor of Arts in History and Politics, first-class honours in Law</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Arts, Law</t>
+          <t>Arts and Law</t>
         </is>
       </c>
     </row>
@@ -817,11 +817,7 @@
           <t>University of Auckland</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>1978</t>
-        </is>
-      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>Arts</t>
@@ -919,7 +915,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Master of Business Administration, Bachelor of Laws</t>
+          <t>Master of Business Administration</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -932,11 +928,7 @@
           <t>1988, unknown</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Business, Law</t>
-        </is>
-      </c>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -986,7 +978,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>1979, 2020</t>
+          <t>1977, 1978, 1979, 2020</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1192,12 +1184,12 @@
           <t>Weltech, Kingston University, Birkbeck, University of London</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Arts, Science, Business</t>
-        </is>
-      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>no specific years mentioned</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1241,7 +1233,11 @@
           <t>University of Waikato, Auckland University of Technology</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>''</t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr">
         <is>
           <t>Arts, Science</t>
@@ -1294,7 +1290,11 @@
           <t>University of Auckland</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
       <c r="K16" t="inlineStr">
         <is>
           <t>Arts, Science</t>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>University of Auckland, Auckland Teachers' Training College, Whangarei Boys' High School, Dargaville High School</t>
+          <t>University of Auckland</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Arts, Law</t>
+          <t>Arts, Science</t>
         </is>
       </c>
     </row>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Victoria University of Wellington, Harvard University</t>
+          <t>Victoria University of Wellington, Harvard Kennedy School at Harvard University</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Bachelor of Commerce</t>
+          <t>Bachelor of Commerce in Accounting and Finance</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1792,11 +1792,7 @@
           <t>Massey University</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>1980s</t>
-        </is>
-      </c>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
           <t>Business</t>
@@ -1856,7 +1852,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Science</t>
+          <t>Arts</t>
         </is>
       </c>
     </row>
@@ -1980,7 +1976,11 @@
           <t>Unitec</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr"/>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
       <c r="K30" t="inlineStr">
         <is>
           <t>Engineering</t>

</xml_diff>